<commit_message>
Doc tags and PCB_Way files
</commit_message>
<xml_diff>
--- a/board/doc/DDT_i2c_proto_breakboard-bom.xlsx
+++ b/board/doc/DDT_i2c_proto_breakboard-bom.xlsx
@@ -134,13 +134,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t/>
+    <t>r1</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2024-08-14_11-03-10</t>
+    <t>2024-08-19</t>
   </si>
   <si>
     <t>KiCad Version:</t>

</xml_diff>